<commit_message>
Login details updated in Test data sheet and share skills edit details entered in share skill excel sheet
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhya\Downloads\MarsFramework\MarsFramework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\IndustryConnect\git\ProjectMarsTestAutomationHybridFramework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA428059-39C0-4B90-8BCF-7E49202B9138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC5064C-28FD-4280-BC04-42A801AF46B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Url</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>http://www.skillswap.pro/Home</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -118,6 +115,15 @@
   </si>
   <si>
     <t>3 years as Oracle Developer and 2 years as Project Management Operations Lead</t>
+  </si>
+  <si>
+    <t>Mars@123</t>
+  </si>
+  <si>
+    <t>archika.mehta19@gmail.com</t>
+  </si>
+  <si>
+    <t>http://192.168.99.100:5000</t>
   </si>
 </sst>
 </file>
@@ -530,36 +536,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -574,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,20 +604,20 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" display="Test@123" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
@@ -622,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -640,66 +646,66 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>